<commit_message>
Wed Nov  8 10:02:21 CST 2023
</commit_message>
<xml_diff>
--- a/笔记/知识点梳理/go.xlsx
+++ b/笔记/知识点梳理/go.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16220"/>
+    <workbookView windowHeight="23420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>问题</t>
   </si>
@@ -63,7 +63,7 @@
     <t>当您为某一类型定义了一个方法，该方法的接收者是这个类型的指针时，那么这个方法只有在这个类型的指针上才能被调用。</t>
   </si>
   <si>
-    <t>示例/go/receiver.go</t>
+    <t>go语言的方法调用过程确实提供了便利性，当你使用一个值类型调用方法时，如果该值类型有一个接收者为指针的方法，Go会自动取该值的地址来调用方法。同样的，如果你有一个指针类型，并且调用的方法接收者是值类型，Go会自动解引用该指针来调用方法。这就是方法调用时的“自动引用/解引用”。</t>
   </si>
   <si>
     <t>值作为接收者声明的方法</t>
@@ -72,10 +72,10 @@
     <t>当您为某一类型定义了一个方法，且该方法的接收者是这个类型的值时，该方法可以在该类型的值和指针上被调用。</t>
   </si>
   <si>
-    <t>切片 和 数组</t>
-  </si>
-  <si>
     <t>切片</t>
+  </si>
+  <si>
+    <t>长度和容量可变</t>
   </si>
   <si>
     <t>切片的长度和容量是可以变的。你可以向切片添加元素（使其增长），也可以删除元素。初始时，上面声明的切片的长度和容量都是0。切片是对底层数组的引用，它可以动态地增长和缩小。
@@ -88,7 +88,63 @@
     <t>var sli []int = make([]int, 5, 10)  // 声明一个长度为5、容量为10的切片</t>
   </si>
   <si>
+    <t>长度和容量定义</t>
+  </si>
+  <si>
+    <t>长度表示你可以操作的元素数量，而容量表示切片背后的数组可以容纳元素的数量。在切片的容量被填满之前，你可以继续向切片追加元素而不会发生重新分配内存。一旦超过容量，追加操作会导致创建一个新的更大的数组，并将原有元素复制到这个新数组中。</t>
+  </si>
+  <si>
+    <t>引用类型</t>
+  </si>
+  <si>
+    <r>
+      <t>切片是引用类型</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，并且当你将一个切片赋值给另一个切片时，它们都将引用同一底层数组的数据。
+64 位架构的机器上，一个切片需要 24 字节的内存：指针字段需要 8 字节，长度和容量
+字段分别需要 8 字节。由于与切片关联的数据包含在底层数组里，不属于切片本身，所以将切片
+复制到任意函数的时候，对底层数组大小都不会有影响。复制时只会复制切片本身，不会涉及底
+层数组</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> slice1 := []int{1, 2, 3}
+ slice2 := slice1 // slice2现在引用与slice1相同的底层数组
+slice2[0] = 10   // 修改slice2的第一个元素也会影响slice1
+// 输出两个切片的内容
+fmt.Println("slice1:", slice1) // slice1: [10 2 3]
+fmt.Println("slice2:", slice2) // slice2: [10 2 3]</t>
+  </si>
+  <si>
+    <t>slice[i:j:k]</t>
+  </si>
+  <si>
+    <t>在Go中，切片表达式 source[2:3:4] 使用了一个全切片操作（full slice expression），它在创建切片时指定了开始索引、结束索引和容量上限。这个表达式创建的新切片将引用原始 source 切片的一部分，具体含义如下：
+2 是新切片的开始索引，新切片将从 source 的第三个元素开始（因为索引从0开始计数）。
+3 是结束索引，新切片将包含 source 直到但不包括索引为3的元素。因此，新切片将只包含一个元素，即 source 的第三个元素。
+4 是新切片的容量上限，它限制了新切片背后的底层数组的容量到原始 source 切片的第四个元素为止。换句话说，尽管 source[2:3] 本身会有更多的可用容量，但是通过指定 4 作为上限，你限制了新切片的容量为2（即 4 - 2）</t>
+  </si>
+  <si>
+    <t>append</t>
+  </si>
+  <si>
+    <t>函数 append 会智能地处理底层数组的容量增长。在切片的容量小于 1000 个元素时，总是
+会成倍地增加容量。一旦元素个数超过 1000，容量的增长因子会设为 1.25，也就是会每次增加 25%
+的容量。随着语言的演化，这种增长算法可能会有所改变</t>
+  </si>
+  <si>
     <t>数组</t>
+  </si>
+  <si>
+    <t>长度固定</t>
   </si>
   <si>
     <t>数组的长度是固定的，它在声明时就确定了。在上面的例子中，array 的长度为5，你不能向其添加第六个元素。
@@ -101,7 +157,147 @@
     <t>var arr [5]int             // 声明一个长度为5的数组</t>
   </si>
   <si>
+    <t>访问速度快</t>
+  </si>
+  <si>
     <t>数组的类型信息可以提供每次访问一个元素时需要在内存中移动的距离。既然数组的每个元素类型相同，又是连续分配，就可以以固定速度索引数组中的任意数据，速度非常快。</t>
+  </si>
+  <si>
+    <t>值类型</t>
+  </si>
+  <si>
+    <r>
+      <t>数组是值类型</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，不是引用类型</t>
+    </r>
+  </si>
+  <si>
+    <t>array1 := [3]int{1, 2, 3}
+array2 := array1 // 复制array1的值到array2
+array2[0] = 10   // 只修改array2的第一个元素
+// 输出两个数组的内容
+fmt.Println("array1:", array1) // array1: [1 2 3]
+ fmt.Println("array2:", array2) // array2: [10 2 3]</t>
+  </si>
+  <si>
+    <t>map</t>
+  </si>
+  <si>
+    <t>无序</t>
+  </si>
+  <si>
+    <t>映射是无序的集合，意味着没有办法预测键值对被返回的顺序。即便使用同样的顺序保存键值对，每次迭代映
+射的时候顺序也可能不一样。无序的原因是映射的实现使用了散列表</t>
+  </si>
+  <si>
+    <t>内存存储原理</t>
+  </si>
+  <si>
+    <r>
+      <t>数组（用于选择桶）：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+映射的第一个数据结构是一个数组，它存储的是</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>散列键的高位值</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">。具体来说，这个数组不直接存储桶，而是存储指向桶的指针或索引。键的散列值的高位被用于快速选择桶。由于这个数组的每个元素大小固定，因此它能够快速地定位到对应的桶。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>桶（buckets）</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>：
+桶本身是第二个数据结构。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>散列键的低位值</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">，通常是一个字节数组。桶内部依次存储了所有的键，紧接着是对应的所有值。存储键和值的方式是连续的，这样可以减少内存碎片，并且在遍历桶内元素时可以提供更好的缓存一致性，因为连续的内存区域往往可以更好地利用CPU缓存。
+这种结构的一个优点是它减少了每个键值对所需的指针数量，因为键和值是紧凑存储的。这种设计在键和值都比较小的情况下内存效率更高。另一个优点是，由于键在桶中是连续存储的，所以在遍历键时可以更有效地利用CPU缓存，这可能提高了遍历速度。
+为了处理散列冲突，每个桶可能会有一个链表或者是一个溢出区域，用于存储那些散列值相同的键。
+</t>
+    </r>
+  </si>
+  <si>
+    <t>interface</t>
+  </si>
+  <si>
+    <t>iTable</t>
+  </si>
+  <si>
+    <t>接口的实现是通过一个内部数据结构，通常被称为iTable（接口表），来完成的。iTable是一个隐含的表结构，它存储了关于接口值的类型信息以及与类型相关的方法集的实现。</t>
+  </si>
+  <si>
+    <t>1. 类型指针：这是一个指向表示接口值动态类型的数据结构的指针。这个类型指针指向的数据结构包含了类型的元数据，如类型的名称、大小、对齐要求等。</t>
+  </si>
+  <si>
+    <t>2. 方法集指针：这是指向方法列表的指针，其中的每个方法都对应于类型实现的接口方法。这些方法是实际代码的入口点，可以调用接口值的具体类型上的方法。</t>
   </si>
 </sst>
 </file>
@@ -114,7 +310,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +321,21 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -271,6 +482,14 @@
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -626,152 +845,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -793,17 +1012,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1124,10 +1379,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="60" customHeight="1" outlineLevelCol="4"/>
@@ -1136,7 +1393,7 @@
     <col min="2" max="2" width="29.8203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="88.40625" style="2" customWidth="1"/>
     <col min="4" max="4" width="52.34375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.2734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="64.1875" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1202,10 +1459,10 @@
       <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" customHeight="1" spans="1:5">
       <c r="A6" s="4"/>
@@ -1215,14 +1472,14 @@
       <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="10"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" customHeight="1" spans="1:5">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -1236,36 +1493,167 @@
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="4"/>
+      <c r="E8" s="12"/>
+    </row>
+    <row r="9" ht="129" customHeight="1" spans="1:5">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="C9" s="11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" customHeight="1" spans="1:5">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+    </row>
+    <row r="10" customHeight="1" spans="1:5">
+      <c r="A10" s="9"/>
+      <c r="B10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="22"/>
+    </row>
+    <row r="11" ht="268" customHeight="1" spans="1:5">
+      <c r="A11" s="9"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" ht="92" customHeight="1" spans="1:5">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="22"/>
+    </row>
+    <row r="13" customHeight="1" spans="1:5">
+      <c r="A13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:5">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" ht="152" customHeight="1" spans="1:5">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:5">
+      <c r="A16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" ht="310" customHeight="1" spans="1:5">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" customHeight="1" spans="1:5">
+      <c r="A18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" customHeight="1" spans="1:5">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" customHeight="1" spans="1:5">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A20"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Tue Jan 16 13:01:51 CST 2024
</commit_message>
<xml_diff>
--- a/笔记/知识点梳理/go.xlsx
+++ b/笔记/知识点梳理/go.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="23420"/>
+    <workbookView windowHeight="16640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
   <si>
     <t>问题</t>
   </si>
@@ -98,6 +98,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>切片是引用类型</t>
     </r>
     <r>
@@ -116,6 +123,9 @@
     </r>
   </si>
   <si>
+    <t>切片复制的仅仅是切片自身，并不包括底层数组。</t>
+  </si>
+  <si>
     <t xml:space="preserve"> slice1 := []int{1, 2, 3}
  slice2 := slice1 // slice2现在引用与slice1相同的底层数组
 slice2[0] = 10   // 修改slice2的第一个元素也会影响slice1
@@ -167,6 +177,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>数组是值类型</t>
     </r>
     <r>
@@ -203,6 +220,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>数组（用于选择桶）：</t>
     </r>
     <r>
@@ -299,16 +324,246 @@
   <si>
     <t>2. 方法集指针：这是指向方法列表的指针，其中的每个方法都对应于类型实现的接口方法。这些方法是实际代码的入口点，可以调用接口值的具体类型上的方法。</t>
   </si>
+  <si>
+    <t xml:space="preserve"> Go 编译器</t>
+  </si>
+  <si>
+    <t>逃逸分析（escape analysis）</t>
+  </si>
+  <si>
+    <t>逃逸分析的工作是确定变量的分配位置（栈或堆）。如果一个变量在函数外部还有引用，即它“逃逸”了函数的作用域，编译器会在堆上为它分配空间，这样即使函数执行结束，变量的生命周期也可以超出函数的作用域，因为堆上的内存直到没有任何引用时才会被垃圾回收。</t>
+  </si>
+  <si>
+    <t>go build -gcflags="-l -m" (禁止内联)</t>
+  </si>
+  <si>
+    <t>func test() *int {
+    a := 0x100
+    return &amp;a
+}
+func main() {
+    var a *int = test()
+    println(a, *a)
+}</t>
+  </si>
+  <si>
+    <t>函数内联（inline）</t>
+  </si>
+  <si>
+    <t>函数内联是一种编译器优化技术，它将一个函数的代码直接插入到调用它的地方，以减少函数调用的开销。内联可以影响内存分配的位置，因为它改变了代码的结构。</t>
+  </si>
+  <si>
+    <t>go build -gcflags="-m"（默认允许内联）</t>
+  </si>
+  <si>
+    <t>如果 test 函数被内联到 main 函数中，局部变量 a 的生命周期就与 main 函数的生命周期相同了。由于 a 被取地址并返回，它可能会在堆上分配，以保证返回的指针在函数返回后依然有效。然而，如果编译器决定 a 的生命周期不会超出其作用域（即，没有其他对它的引用），那么它可能仍然会在栈上分配。</t>
+  </si>
+  <si>
+    <t>内联优点：
+1. 性能：栈上的内存分配和回收通常只涉及到调整栈指针，这是非常快的操作，而堆上的内存分配和回收则涉及更复杂的内存管理策略，如空闲列表管理，这些操作通常比栈操作要慢。
+2. 内存管理简单：栈内存是自管理的，当函数调用完成后，分配给它的栈内存会自动被回收。相比之下，堆内存需要显式地分配和释放，如果不当管理，会导致内存泄露。
+3. 局部性：栈内存通常用来存储局部变量，这些变量的生命周期较短，且访问频繁，这有利于缓存和快速访问。堆内存分布可能更分散，这可能会影响缓存的效率。
+4. 确定性：栈内存的分配和释放通常具有确定性，便于预测程序的行为。而堆内存的分配可能因为内存碎片化等问题而有不确定的延迟。
+5. 线程安全：每个线程都有自己的栈空间，所以栈上的数据自然地被线程隔离，减少了线程同步的需求。而堆内存是由所有线程共享的，需要额外的同步机制来避免竞争条件。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">尾递归优化 (tail-call optimization. TCO）
+</t>
+  </si>
+  <si>
+    <t>是编译器的一个功能，它能在特定条件下改进递归函数的性能。在尾递归函数中，函数的最后一个操作是调用自身（尾调用），并且不需要保留当前函数的栈帧，因为没有更多的操作需要在返回后执行。</t>
+  </si>
+  <si>
+    <t>func Recur(n int) int {
+    if n &lt;= 1 {
+        return n
+    }
+    return Recur(n - 1)
+}</t>
+  </si>
+  <si>
+    <t>在没有尾调用优化的情况下，每次函数递归调用自身时，都会在调用栈上创建一个新的栈帧，这可能会导致在深度递归时栈溢出。TCO 允许函数在递归调用自身时重用当前的栈帧，因为当前帧在尾调用发生时不再需要了。这样做有效地将递归过程转换成了迭代过程，从而避免了栈溢出，降低了函数调用的开销。</t>
+  </si>
+  <si>
+    <t>在尾递归优化之前，每次调用 Recur 都会增加一个栈帧。如果 n 很大，这可能会导致栈溢出。然而，如果编译器能够识别这种模式，并应用尾递归优化，那么递归调用可以被转换成跳转，重用当前的栈帧而不是创建新的。</t>
+  </si>
+  <si>
+    <t>GO 编译器目前不支持尾递归优化</t>
+  </si>
+  <si>
+    <t>参数</t>
+  </si>
+  <si>
+    <t>不支持实名参数（Named Arguments）</t>
+  </si>
+  <si>
+    <t>不能在调用函数时显式地标明每个参数的名称。相反，你必须按照函数定义时参数的顺序传递参数。</t>
+  </si>
+  <si>
+    <t>myFunc(123, "hello") // 正确的调用方式</t>
+  </si>
+  <si>
+    <t>myFunc(param1: 123, param2: "hello") // 错误的语法</t>
+  </si>
+  <si>
+    <t>变参</t>
+  </si>
+  <si>
+    <t>变参本质上是一个切片</t>
+  </si>
+  <si>
+    <t>func test(s string, a ...int)</t>
+  </si>
+  <si>
+    <t>命名参数</t>
+  </si>
+  <si>
+    <t>可当做函数局部变量使用</t>
+  </si>
+  <si>
+    <t>指针参数导致实参变量被分配到堆上</t>
+  </si>
+  <si>
+    <t>1. 在 main 函数中，变量 x 被分配在 main 的栈帧上，并且其地址被传递给 test 函数。
+2. 在 test 函数中，您启动了一个新的 goroutine，并在这个 goroutine 中使用了 p 指针（这个指针指向 main 中的 x）。
+3. 由于新的 goroutine 可能在 test 函数返回后仍在执行，因此 x 的引用（通过 p 指针）逃逸到了 test 函数之外。这意味着 x 不能仅仅存在于 main 的栈帧上，因为它必须在 test 函数返回后依然可用。
+4. 因此，编译器可能决定将 x 分配到堆上，以确保在 test 函数返回后，新启动的 goroutine 仍然可以安全地访问它。</t>
+  </si>
+  <si>
+    <t>func test(p *int) {
+  go func() {
+   println(p)
+  }()
+}
+func main() {
+ x := 100
+ p := &amp;x
+ test(p)
+}</t>
+  </si>
+  <si>
+    <t>返回值</t>
+  </si>
+  <si>
+    <t>命名返回值</t>
+  </si>
+  <si>
+    <t>函数</t>
+  </si>
+  <si>
+    <t>闭包（Closure）</t>
+  </si>
+  <si>
+    <t>闭包（Closure）是一种特殊的函数，它可以捕获并包含其外部作用域中的变量。闭包通常与匿名函数一起使用，使得你可以在一个函数内部创建另一个函数，后者能够访问并操作前者作用域中的变量。</t>
+  </si>
+  <si>
+    <t>adder 函数返回一个匿名函数，该匿名函数形成了一个闭包</t>
+  </si>
+  <si>
+    <t xml:space="preserve">package main
+import "fmt"
+func main() {
+    adder := func(x int) func(int) int {
+        return func(y int) int {
+            x += y
+            return x
+        }
+    }
+    sum := adder(10)
+    fmt.Println(sum(5))  // 输出：15
+    fmt.Println(sum(10)) // 输出：25
+}
+</t>
+  </si>
+  <si>
+    <t>1. 封装状态：闭包可以用来维护和封装状态。在上面的例子中，闭包 sum 维护了一个累加器的状态。</t>
+  </si>
+  <si>
+    <t>闭包 sum 能够访问并修改其外部函数 adder 的局部变量 x。</t>
+  </si>
+  <si>
+    <t>2. 回调函数：在处理异步操作或设计事件监听器时，闭包常被用作回调函数，因为它们能够访问其他函数的变量。</t>
+  </si>
+  <si>
+    <t>即使在 adder 函数执行完成之后，闭包仍然记住了 x 的值，并能够在随后的调用中使用和修改它。</t>
+  </si>
+  <si>
+    <t>3. 实现函数式编程模式：闭包支持函数式编程中的许多模式，如高阶函数，允许函数操作、返回其他函数等。</t>
+  </si>
+  <si>
+    <t>返回的不仅仅是匿名函数，还有所引用的环境变量的指针。所以匿名函数可以访问并修改它外部作用域的变量。</t>
+  </si>
+  <si>
+    <t>闭包 与 匿名函数</t>
+  </si>
+  <si>
+    <t>在 Go 中，所有匿名函数都可以访问它们外部作用域的变量，因此它们都可以形成闭包。</t>
+  </si>
+  <si>
+    <t>当匿名函数利用了其能夠访问外部作用域变量的能力时，它就形成了闭包。</t>
+  </si>
+  <si>
+    <t>defer</t>
+  </si>
+  <si>
+    <t>多个延迟注册按 FILO 次序执行</t>
+  </si>
+  <si>
+    <t>defer println("a")
+defer println("b")
+输出:
+b
+a</t>
+  </si>
+  <si>
+    <t>相比直接调用 CALL 汇编指令调用函数，延迟调用须花费更大代价。包括注册，调用等操作。还有额外的缓存开销。</t>
+  </si>
+  <si>
+    <t>painc, recover</t>
+  </si>
+  <si>
+    <t>连续调用panic, 仅最后一个会被 recover 捕获</t>
+  </si>
+  <si>
+    <t>数据</t>
+  </si>
+  <si>
+    <t>字符串</t>
+  </si>
+  <si>
+    <t>字符串底层是以字节序列的形式存储的。可以通过索引来访问字符串中的单个字节，就像访问数组或切片中的元素一样。</t>
+  </si>
+  <si>
+    <t>尽管可以访问字符串中的字节，但不能直接获取字符串元素的地址。这是因为：
+1. 不可变性：字符串在 Go 中是不可变的。如果能够获取字符串元素的地址，就可能导致通过该地址修改字符串的内容，这与字符串的不可变性相冲突。
+2. 安全性：不允许直接访问字符串内部数据的地址，是一种安全措施，以防止程序意外或恶意地更改字符串的内容。</t>
+  </si>
+  <si>
+    <t>reflect.StringHeader</t>
+  </si>
+  <si>
+    <t>reflect.StringHeader 是一个结构体，用于表示字符串的内部表示。这个结构体提供了底层字符串的详细信息</t>
+  </si>
+  <si>
+    <t>type StringHeader struct {
+    Data uintptr
+    Len  int
+}</t>
+  </si>
+  <si>
+    <t>1. Data 字段是一个 uintptr 类型，它存储了字符串实际数据的地址。这个地址指向字符串的第一个字节。
+2. Len 字段是一个 int 类型，表示字符串的长度，即字符串中的字节总数。</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -349,6 +604,84 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -357,100 +690,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -465,14 +706,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -480,6 +714,27 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -508,192 +763,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -743,17 +998,41 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -763,6 +1042,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -797,13 +1085,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -819,24 +1111,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -845,152 +1124,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1018,40 +1297,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1063,54 +1345,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
     <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1379,19 +1661,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18:E20"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="60" customHeight="1" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="32.6796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.8203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="88.40625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="89.96875" style="2" customWidth="1"/>
     <col min="4" max="4" width="52.34375" style="1" customWidth="1"/>
     <col min="5" max="5" width="64.1875" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
@@ -1462,7 +1744,7 @@
       <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="20"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" customHeight="1" spans="1:5">
       <c r="A6" s="4"/>
@@ -1473,13 +1755,13 @@
         <v>17</v>
       </c>
       <c r="D6" s="8"/>
-      <c r="E6" s="21"/>
+      <c r="E6" s="13"/>
     </row>
     <row r="7" customHeight="1" spans="1:5">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -1493,168 +1775,516 @@
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="12"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" ht="129" customHeight="1" spans="1:5">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="22" t="s">
+      <c r="D9" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="E9" s="23" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" customHeight="1" spans="1:5">
-      <c r="A10" s="9"/>
-      <c r="B10" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="A10" s="4"/>
+      <c r="B10" s="11" t="s">
         <v>29</v>
       </c>
+      <c r="C10" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="22"/>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" ht="268" customHeight="1" spans="1:5">
-      <c r="A11" s="9"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="22"/>
+      <c r="E11" s="23"/>
     </row>
     <row r="12" ht="92" customHeight="1" spans="1:5">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="15" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="C12" s="14" t="s">
+        <v>32</v>
+      </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="22"/>
+      <c r="E12" s="23"/>
     </row>
     <row r="13" customHeight="1" spans="1:5">
-      <c r="A13" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="B13" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="C13" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:5">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="16" t="s">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="C14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" ht="152" customHeight="1" spans="1:5">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="17" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="16" t="s">
+      <c r="C15" s="10" t="s">
         <v>41</v>
       </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" customHeight="1" spans="1:5">
-      <c r="A16" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="B16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
+      <c r="C16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" ht="310" customHeight="1" spans="1:5">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="18" t="s">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
+      <c r="C17" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" customHeight="1" spans="1:5">
-      <c r="A18" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="B18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="C18" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" customHeight="1" spans="1:5">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" customHeight="1" spans="1:5">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" customHeight="1" spans="1:5">
+      <c r="A21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="1:5">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" customHeight="1" spans="1:5">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" ht="189" customHeight="1" spans="1:5">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" customHeight="1" spans="1:5">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" customHeight="1" spans="1:5">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" customHeight="1" spans="1:5">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" customHeight="1" spans="1:5">
+      <c r="A28" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" customHeight="1" spans="1:5">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" customHeight="1" spans="1:5">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" customHeight="1" spans="1:5">
+      <c r="A31" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" customHeight="1" spans="1:5">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" customHeight="1" spans="1:5">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" customHeight="1" spans="1:5">
+      <c r="A34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" customHeight="1" spans="1:5">
+      <c r="A35" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" customHeight="1" spans="1:5">
+      <c r="A36" s="21"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36" s="20"/>
+    </row>
+    <row r="37" customHeight="1" spans="1:5">
+      <c r="A37" s="21"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="20"/>
+    </row>
+    <row r="38" customHeight="1" spans="1:5">
+      <c r="A38" s="21"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="19"/>
+      <c r="E38" s="20"/>
+    </row>
+    <row r="39" customHeight="1" spans="1:5">
+      <c r="A39" s="21"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+    </row>
+    <row r="40" customHeight="1" spans="1:5">
+      <c r="A40" s="21"/>
+      <c r="B40" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+    </row>
+    <row r="41" customHeight="1" spans="1:5">
+      <c r="A41" s="21"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+    </row>
+    <row r="42" customHeight="1" spans="1:5">
+      <c r="A42" s="21"/>
+      <c r="B42" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D42" s="19"/>
+      <c r="E42" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" customHeight="1" spans="1:5">
+      <c r="A43" s="21"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="19"/>
+      <c r="E43" s="20"/>
+    </row>
+    <row r="44" customHeight="1" spans="1:5">
+      <c r="A44" s="22"/>
+      <c r="B44" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+    </row>
+    <row r="45" customHeight="1" spans="1:5">
+      <c r="A45" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+    </row>
+    <row r="46" customHeight="1" spans="1:5">
+      <c r="A46" s="19"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+    </row>
+    <row r="47" customHeight="1" spans="1:5">
+      <c r="A47" s="19"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+    </row>
+    <row r="48" customHeight="1" spans="1:5">
+      <c r="A48" s="19"/>
+      <c r="B48" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" s="19"/>
+      <c r="E48" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" customHeight="1" spans="1:5">
+      <c r="A49" s="19"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D49" s="19"/>
+      <c r="E49" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="33">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A35:A44"/>
+    <mergeCell ref="A45:A49"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B35:B39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B49"/>
     <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="C46:C47"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="E31:E33"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="E48:E49"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Sun 19 Jan 2025 13:32:55 CST
</commit_message>
<xml_diff>
--- a/笔记/知识点梳理/go.xlsx
+++ b/笔记/知识点梳理/go.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="186">
   <si>
     <t>问题</t>
   </si>
@@ -25,7 +25,7 @@
     <t>说明</t>
   </si>
   <si>
-    <t>建议</t>
+    <t>备注</t>
   </si>
   <si>
     <t>样例</t>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>切片</t>
+  </si>
+  <si>
+    <t>创建切片</t>
+  </si>
+  <si>
+    <t>创建切片对象，无须预先准备数组。因为是引用类型，须使用 make 函数或显示初始化语句，它会自动完成底层数组内存分配。</t>
   </si>
   <si>
     <t>长度和容量可变</t>
@@ -123,7 +129,8 @@
     </r>
   </si>
   <si>
-    <t>切片复制的仅仅是切片自身，并不包括底层数组。</t>
+    <t>切片复制的仅仅是切片自身，并不包括底层数组。
+切片本身是个只读对象，其工作机制类似数组指针的一种包装。</t>
   </si>
   <si>
     <t xml:space="preserve"> slice1 := []int{1, 2, 3}
@@ -149,6 +156,15 @@
     <t>函数 append 会智能地处理底层数组的容量增长。在切片的容量小于 1000 个元素时，总是
 会成倍地增加容量。一旦元素个数超过 1000，容量的增长因子会设为 1.25，也就是会每次增加 25%
 的容量。随着语言的演化，这种增长算法可能会有所改变</t>
+  </si>
+  <si>
+    <t>数据被追加到原底层数组。如超出 cap 限制，则为新切片对象重新分配数组。</t>
+  </si>
+  <si>
+    <t>切片 vs 数组</t>
+  </si>
+  <si>
+    <t>切片只是很小的结构体对象，用来代替数组传参可以避免复制开销。</t>
   </si>
   <si>
     <t>数组</t>
@@ -194,7 +210,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>，不是引用类型</t>
+      <t>，不是引用类型。</t>
     </r>
   </si>
   <si>
@@ -203,7 +219,19 @@
 array2[0] = 10   // 只修改array2的第一个元素
 // 输出两个数组的内容
 fmt.Println("array1:", array1) // array1: [1 2 3]
- fmt.Println("array2:", array2) // array2: [10 2 3]</t>
+fmt.Println("array2:", array2) // array2: [10 2 3]</t>
+  </si>
+  <si>
+    <t>比较</t>
+  </si>
+  <si>
+    <t>数组可以使用 == 进行比较，前提是它们的类型完全相同（即元素类型和数组长度都相同）。当使用 == 对数组进行比较时，Go 会逐个比较数组中对应位置的元素，所有元素都相等时，两个数组才被认为是相等的。</t>
+  </si>
+  <si>
+    <t>操作与赋值</t>
+  </si>
+  <si>
+    <t>Go 数组是值类型，赋值和操作都会复制整个数组。</t>
   </si>
   <si>
     <t>map</t>
@@ -212,8 +240,117 @@
     <t>无序</t>
   </si>
   <si>
-    <t>映射是无序的集合，意味着没有办法预测键值对被返回的顺序。即便使用同样的顺序保存键值对，每次迭代映
-射的时候顺序也可能不一样。无序的原因是映射的实现使用了散列表</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>映射是无序的集合，意味着没有办法预测键值对被返回的顺序。即便使用同样的顺序保存键值对，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>每次迭代映
+射的时候顺序也可能不一样</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>。无序的原因是映射的实现使用了散列表</t>
+    </r>
+  </si>
+  <si>
+    <t>修改</t>
+  </si>
+  <si>
+    <t>因内存访问安全和哈希算法等缘故，字典被设计成 "not addressable"，不能直接修改 value 成员（结构或数组）。</t>
+  </si>
+  <si>
+    <t>1. 返回整个value, 待修改后再设置字典键值，或直接用指针类型
+2. 直接使用指针类型</t>
+  </si>
+  <si>
+    <t>m := map[int]user{xxx}
+m[1].age += 1 // 不能直接修改
+m := map[int]*user{xxx}
+m[1].apge += 1 // 可以修改</t>
+  </si>
+  <si>
+    <t>并发检测</t>
+  </si>
+  <si>
+    <t>运行时会对字典并发操作做出检测。如果某个任务正在对字典进行写操作，那么其他任务就不能对该字典执行并发操作（读、写、删除），否则会导致进程崩溃。</t>
+  </si>
+  <si>
+    <t>传参</t>
+  </si>
+  <si>
+    <t>字典对象本身就是指针包装，传参时无需再次取地址。</t>
+  </si>
+  <si>
+    <t>小对象存储设计</t>
+  </si>
+  <si>
+    <t>对于海量小对象，应直接用字典存储键值数据拷贝，而非指针。有助于减少需要扫描的对象数量，大幅缩短垃圾回收时间。另外，字典不会收缩内存，所以适当替换成新对象是必要的。</t>
+  </si>
+  <si>
+    <t>不收缩内存</t>
+  </si>
+  <si>
+    <t>在 Go 语言中，map（字典）在增长以容纳更多元素时会自动增加其内存使用量，以保持其性能。这种设计允许快速的查找、添加和删除操作。然而，即使从字典中删除了许多元素，Go 的字典结构也不会自动减少其占用的内存空间（即不会自动收缩），因为标准的 Go 语言运行时不提供显式的方式来减小已分配的内存大小。
+因此，如果你有一个大字典，并且从中删除了大量的元素，留下了许多未使用的空间，这个字典仍然会占用当初分配给它的内存空间。在长期运行的应用程序中，这可能导致不必要的内存使用，甚至内存泄漏。
+为了管理这种情况，如果你知道字典已经不再需要存储许多元素，一种常见的做法是手动替换掉原有的字典。这可以通过创建一个新的字典对象并将旧字典中仍需要保留的元素复制过去来完成。这样做可以释放掉原字典占用的大量内存，因为新的字典将只占用必要的更小内存空间。</t>
+  </si>
+  <si>
+    <t>map类型的值不能直接使用==操作符来进行比较。这是因为map是一个引用类型，而==用于比较两个值是否相同。对于大多数引用类型（如slices, maps, 和functions），Go不允许使用==操作符进行直接比较，主要是因为比较这些类型的内存地址是否相同通常没有实际意义。特别是对于map，比较的意图通常是判断两个map是否含有相同的键值对，而这涉及到对map内部元素的深度比较，这不是==操作符所能提供的。</t>
+  </si>
+  <si>
+    <t>分配</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>在创建时</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>预先准备足够空间</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>有助于提升性能，减少扩张时的内存分配和重新哈希操作。</t>
+    </r>
   </si>
   <si>
     <t>内存存储原理</t>
@@ -310,6 +447,68 @@
     </r>
   </si>
   <si>
+    <t>通过键从一个映射中检索值时，如果映射的值是一个数组类型，你得到的是该数组值的一个副本，而不是原始数组的引用。</t>
+  </si>
+  <si>
+    <t>m := map[string][2]int{ "a": {1,2}}
+s := m["a"][:] // 提示 m["a"][:] slice of unaddressable value</t>
+  </si>
+  <si>
+    <t>结构体</t>
+  </si>
+  <si>
+    <t>定义</t>
+  </si>
+  <si>
+    <t>结构体将多个不同类型命名字段（field）序列打包成一个复合类型。</t>
+  </si>
+  <si>
+    <t>除对齐处理外，编译器不会优化，调整内存布局。具体针对结构体中的字段与对其的影响，查看示例。</t>
+  </si>
+  <si>
+    <t>查看 示例/align.go</t>
+  </si>
+  <si>
+    <t>空结构体</t>
+  </si>
+  <si>
+    <t>"长度"为零的对象都指向 runtime.zerobase 变量</t>
+  </si>
+  <si>
+    <t>var d [100]struct{}</t>
+  </si>
+  <si>
+    <t>空结构体（struct{}）可以作为通道的元素类型，即chan struct{}</t>
+  </si>
+  <si>
+    <t>struct{}类型的大小为0，因此chan struct{}用于事件通知时，相比于其他数据类型的通道更节省内存。
+使用chan struct{}作为信号通道，明确表示通道不会被用于传递数据，只用于事件的同步或通知，增强了代码的可读性。</t>
+  </si>
+  <si>
+    <t>对齐</t>
+  </si>
+  <si>
+    <t>分配内存时，字段必须对齐处理，通常以所有字段中最长的基础类型宽度为标准。</t>
+  </si>
+  <si>
+    <t>右边代码的对其宽度为8, 取 基础类型 int。
+结构体的 size 为 40
+1. a byte: 对齐后为8
+2. b []int: slice  包括 ptr, len, cap size为 24
+3. c byte: 对齐后为8</t>
+  </si>
+  <si>
+    <t>v3 := struct{ 
+  a byte
+  b []int
+  c byte
+}{}</t>
+  </si>
+  <si>
+    <t>如果空结构类型字段是最后一个字段，编译器将其当做长度为1的类型做对齐处理，以便其地址不会越界，避免引发垃圾回收错误。
+如果仅有一个空结构字段，那么同样按1对齐，只不过长度为0，且指向 runtime.zerobase 变量</t>
+  </si>
+  <si>
     <t>interface</t>
   </si>
   <si>
@@ -525,7 +724,7 @@
     <t>连续调用panic, 仅最后一个会被 recover 捕获</t>
   </si>
   <si>
-    <t>数据</t>
+    <t>string</t>
   </si>
   <si>
     <t>字符串</t>
@@ -553,6 +752,127 @@
   <si>
     <t>1. Data 字段是一个 uintptr 类型，它存储了字符串实际数据的地址。这个地址指向字符串的第一个字节。
 2. Len 字段是一个 int 类型，表示字符串的长度，即字符串中的字节总数。</t>
+  </si>
+  <si>
+    <t>string 与 []byte 非安全转换</t>
+  </si>
+  <si>
+    <t>通过 Go 语言中的非安全（unsafe）包来实现 []byte 到 string 的转换，利用的是 []byte 和 string 在内存中的表现形式有部分相似性，特别是它们的头部结构。这种方法绕过了 Go 的类型安全机制，直接在底层内存表示上操作，因此被称为"非安全"的。</t>
+  </si>
+  <si>
+    <t>1. unsafe.Pointer(&amp;bs)：首先，我们取得 bs（[]byte 类型的变量）的地址，并将这个地址转换为 unsafe.Pointer。这是一种特殊的指针类型，允许我们绕过 Go 的类型系统。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">func toString(bs []byte) string {
+  return *(*string)(unsafe.Pointer(&amp;bs))
+}
+</t>
+  </si>
+  <si>
+    <t>在 Go 语言中，string 和 []byte 都是对底层数据的引用，但它们的处理方式有所不同。string 是不可变的，而 []byte 是可变的。尽管它们在内存中的表示方式有所不同，但它们都包含指向数据存储位置的指针和数据长度信息。这是它们相似的地方。</t>
+  </si>
+  <si>
+    <t>2. (*string)(unsafe.Pointer(&amp;bs))：接着，我们将 unsafe.Pointer 转换为 *string 类型，也就是指向 string 的指针。这一步假定 []byte 的内存布局与 string 兼容，尽管实际上它们的内部表示有区别。这个转换并没有改变内存中的数据，只是改变了我们访问这些数据的方式。</t>
+  </si>
+  <si>
+    <t>它们的兼容性来自于前两个字段的相似性——即指向数据的指针和数据长度。这两个类型的前两个字段（指针和长度）在内存布局上是一致的。因此，通过非安全的操作，可以在这两种类型之间进行转换而不改变底层数据。</t>
+  </si>
+  <si>
+    <t>3. *(*string)(unsafe.Pointer(&amp;bs))：最后，我们通过解引用操作符 * 来获取指针指向的值，也就完成了从 []byte 到 string 的转换。</t>
+  </si>
+  <si>
+    <t>string 内存布局</t>
+  </si>
+  <si>
+    <t>string 被表示为一个结构体，这个结构体有两个字段：
+1. 指针 (ptr)：指向实际字符串数据的起始位置。这部分数据是不可变的。
+2. 长度 (len)：表示字符串的长度（以字节为单位），不是字符数。这是因为 Go 的字符串是 UTF-8 编码的，一个字符可能会占用多个字节。</t>
+  </si>
+  <si>
+    <t>当我们通过 unsafe 包实现 []byte 到 string 的转换时，实际上是在告诉编译器将 []byte 结构体视为 string 结构体。因为 string 和 []byte 的前两个字段（指针和长度）在内存中的布局是一致的，这种转换在技术上是可行的。但请注意，这种操作跳过了 Go 的类型安全检查，可能会引入潜在的安全风险。</t>
+  </si>
+  <si>
+    <t>[]byte 的内存布局</t>
+  </si>
+  <si>
+    <t>1. 指针 (ptr)：指向切片底层数组中数据的起始位置。
+2. 长度 (len)：切片中的元素数量。
+3. 容量 (cap)：从切片的起始元素到底层数组末尾的元素数量。这允许切片动态增长，直到达到底层数组的大小。</t>
+  </si>
+  <si>
+    <t>方法</t>
+  </si>
+  <si>
+    <t>方法是与对象实例绑定的特殊函数。</t>
+  </si>
+  <si>
+    <t>方法与函数</t>
+  </si>
+  <si>
+    <t>方法是有关联状态的，函数通常没有。</t>
+  </si>
+  <si>
+    <t>接口</t>
+  </si>
+  <si>
+    <t>实现方式</t>
+  </si>
+  <si>
+    <t>只要目标类型方法集内包含接口声明的全部方法，就被视为实现了该接口，无须做显示声明。目标类型可以是实现多个接口。</t>
+  </si>
+  <si>
+    <t>匿名接口</t>
+  </si>
+  <si>
+    <t>匿名接口最常见的形式是interface{}，它是一个空接口，没有定义任何方法。由于在Go中接口是隐式实现的，任何类型都至少实现了零个方法，因此任何类型都实现了interface{}。这使得interface{}可以用来表示任意类型的值，提供极大的灵活性。但除了interface{}外，匿名接口还可以在定义更具体的行为时使用，尽管这种用法不如interface{}普遍。</t>
+  </si>
+  <si>
+    <t>1. 作为函数参数或返回值，简化代码：在需要传递带有特定方法集的类型时，匿名接口允许直接在函数签名中声明这些方法，避免创建一个具名接口。这可以使代码更加简洁，尤其是在接口仅在一个小的作用域内部使用时。</t>
+  </si>
+  <si>
+    <t>func processItems(items []interface{ process() error })</t>
+  </si>
+  <si>
+    <t>2. 临时组合多个接口： 在某些情况下，你可能需要一个函数接受实现了多个接口的类型作为参数。使用匿名接口可以临时创建一个组合接口，而不需要定义一个新的具名接口。</t>
+  </si>
+  <si>
+    <t>func performAction(item interface{ read(); write() })</t>
+  </si>
+  <si>
+    <t>执行机制</t>
+  </si>
+  <si>
+    <t>接口的工作机制依赖于一些内部数据结构，其中iface和itab是两个核心的结构体。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iface是表示接口值的内部结构体。在Go语言的运行时系统中，每个接口值都由一个iface结构体实例表示。这个结构体包含两个主要的字段:
+1. tab：指向itab结构体的指针。itab结构体包含了接口类型和具体类型之间的映射信息，以及具体类型实现的接口方法的函数指针
+2. data：一个指向实际数据（具体类型的值）的指针。这是一个unsafe.Pointer，因为Go语言的接口可以持有任何类型的值，所以这里需要一个通用的指针类型来表示任意的数据。
+</t>
+  </si>
+  <si>
+    <t>当一个具体类型的值被赋给一个接口类型的变量时，Go运行时会创建或查找一个itab实例，来记录这个具体类型是如何实现该接口的。接着，运行时创建一个iface实例，其tab字段指向itab，而data字段指向具体的值。通过这种方式，接口值知道了如何找到并调用其方法。
+例如，当你调用一个接口的方法时，Go运行时会首先查找iface结构体的tab字段，找到对应的itab，然后通过itab中的fun数组找到具体实现的方法，最后使用data字段作为接收者调用该方法。</t>
+  </si>
+  <si>
+    <t>type iface struct {
+ tab *itab     //类型信息
+ data unsafe.Pointer  //实际对象指针
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type itab struct {
+ inter *interfacetype //接口类型
+ _type *_type   //实际对象类型
+ fun [1]uintptr   //实际对象方法地址
+}
+</t>
+  </si>
+  <si>
+    <t>itab是接口表（interface table）的缩写，它是Go运行时用于存储接口与具体类型之间关系的内部结构体。itab的存在使得接口方法的动态调用成为可能。它包含以下字段：
+1. inter：指向interfacetype结构体的指针，这个结构体描述了接口自身的类型信息，比如接口定义的方法集合。
+2. _type：指向_type结构体的指针，这个结构体表示实现了接口的具体类型的类型信息。
+3. fun：这是一个函数指针的数组。数组中的每一个元素都对应于接口定义的一个方法。这些函数指针指向具体类型实现这些接口方法的具体函数。</t>
   </si>
 </sst>
 </file>
@@ -565,7 +885,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -740,6 +1060,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
@@ -998,6 +1325,17 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -1008,17 +1346,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1269,7 +1596,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1292,55 +1619,64 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1661,20 +1997,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomLeft" activeCell="B84" sqref="B84:C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="60" customHeight="1" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="32.6796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.8203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="89.96875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="52.34375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="94.7890625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="69.5234375" style="1" customWidth="1"/>
     <col min="5" max="5" width="64.1875" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
@@ -1732,7 +2068,7 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" customHeight="1" spans="1:5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -1741,24 +2077,24 @@
       <c r="C5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" customHeight="1" spans="1:5">
-      <c r="A6" s="4"/>
+      <c r="A6" s="9"/>
       <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="13"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" customHeight="1" spans="1:5">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1767,524 +2103,933 @@
       <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" customHeight="1" spans="1:5">
+      <c r="A8" s="11"/>
+      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" customHeight="1" spans="1:5">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" ht="129" customHeight="1" spans="1:5">
-      <c r="A9" s="4"/>
-      <c r="B9" s="9" t="s">
+    </row>
+    <row r="9" customHeight="1" spans="1:5">
+      <c r="A9" s="11"/>
+      <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" ht="129" customHeight="1" spans="1:5">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="C10" s="13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" customHeight="1" spans="1:5">
-      <c r="A10" s="4"/>
-      <c r="B10" s="11" t="s">
+      <c r="D10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="E10" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="23"/>
-    </row>
-    <row r="11" ht="268" customHeight="1" spans="1:5">
-      <c r="A11" s="4"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="23"/>
-    </row>
-    <row r="12" ht="92" customHeight="1" spans="1:5">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4" t="s">
+    </row>
+    <row r="11" customHeight="1" spans="1:5">
+      <c r="A11" s="11"/>
+      <c r="B11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="23"/>
-    </row>
-    <row r="13" customHeight="1" spans="1:5">
-      <c r="A13" s="4" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" ht="205" customHeight="1" spans="1:5">
+      <c r="A12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" ht="92" customHeight="1" spans="1:5">
+      <c r="A13" s="11"/>
+      <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" ht="59" customHeight="1" spans="1:5">
+      <c r="A14" s="11"/>
+      <c r="B14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="C14" s="15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" customHeight="1" spans="1:5">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" customHeight="1" spans="1:5">
+      <c r="A15" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" ht="152" customHeight="1" spans="1:5">
-      <c r="A15" s="4"/>
-      <c r="B15" s="9" t="s">
+      <c r="C15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:5">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="11"/>
+      <c r="B16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" ht="310" customHeight="1" spans="1:5">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4" t="s">
+    <row r="17" ht="130" customHeight="1" spans="1:5">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="4"/>
+      <c r="E17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" customHeight="1" spans="1:5">
-      <c r="A18" s="4" t="s">
+    </row>
+    <row r="18" ht="127" customHeight="1" spans="1:5">
+      <c r="A18" s="11"/>
+      <c r="B18" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" ht="81" customHeight="1" spans="1:5">
+      <c r="A19" s="9"/>
+      <c r="B19" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-    </row>
-    <row r="19" customHeight="1" spans="1:5">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="17" t="s">
         <v>51</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" customHeight="1" spans="1:5">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>52</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>54</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" customHeight="1" spans="1:5">
-      <c r="A21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="6" t="s">
+    <row r="21" ht="85" customHeight="1" spans="1:5">
+      <c r="A21" s="11"/>
+      <c r="B21" s="7" t="s">
         <v>55</v>
       </c>
+      <c r="C21" s="17" t="s">
+        <v>56</v>
+      </c>
       <c r="D21" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" customHeight="1" spans="1:5">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="6" t="s">
+    </row>
+    <row r="22" ht="77" customHeight="1" spans="1:5">
+      <c r="A22" s="11"/>
+      <c r="B22" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="C22" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" customHeight="1" spans="1:5">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="6" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" ht="77" customHeight="1" spans="1:5">
+      <c r="A23" s="11"/>
+      <c r="B23" s="7" t="s">
         <v>61</v>
       </c>
+      <c r="C23" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="D23" s="4"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" ht="189" customHeight="1" spans="1:5">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5" t="s">
-        <v>62</v>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" ht="77" customHeight="1" spans="1:5">
+      <c r="A24" s="11"/>
+      <c r="B24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>64</v>
       </c>
       <c r="D24" s="4"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" customHeight="1" spans="1:5">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>64</v>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" ht="175" customHeight="1" spans="1:5">
+      <c r="A25" s="11"/>
+      <c r="B25" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>66</v>
       </c>
       <c r="D25" s="4"/>
-      <c r="E25" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" customHeight="1" spans="1:5">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="6" t="s">
-        <v>66</v>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" ht="87" customHeight="1" spans="1:5">
+      <c r="A26" s="11"/>
+      <c r="B26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" customHeight="1" spans="1:5">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" ht="77" customHeight="1" spans="1:5">
+      <c r="A27" s="11"/>
+      <c r="B27" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" customHeight="1" spans="1:5">
-      <c r="A28" s="4" t="s">
+      <c r="C27" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" ht="310" customHeight="1" spans="1:5">
+      <c r="A28" s="11"/>
+      <c r="B28" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" ht="71" customHeight="1" spans="1:5">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="D29" s="4"/>
+      <c r="E29" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" customHeight="1" spans="1:5">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4" t="s">
+    <row r="30" ht="71" customHeight="1" spans="1:5">
+      <c r="A30" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="B30" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4" t="s">
+      <c r="C30" s="18" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="30" customHeight="1" spans="1:5">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="E30" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-    </row>
-    <row r="31" customHeight="1" spans="1:5">
-      <c r="A31" s="4" t="s">
+    </row>
+    <row r="31" ht="71" customHeight="1" spans="1:5">
+      <c r="A31" s="11"/>
+      <c r="B31" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="6" t="s">
+      <c r="D31" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" customHeight="1" spans="1:5">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" customHeight="1" spans="1:5">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" customHeight="1" spans="1:5">
-      <c r="A34" s="4" t="s">
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" ht="71" customHeight="1" spans="1:5">
+      <c r="A32" s="11"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>78</v>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" ht="95" customHeight="1" spans="1:5">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" ht="71" customHeight="1" spans="1:5">
+      <c r="A34" s="9"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="E34" s="5"/>
     </row>
     <row r="35" customHeight="1" spans="1:5">
-      <c r="A35" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>88</v>
-      </c>
+      <c r="A35" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" customHeight="1" spans="1:5">
-      <c r="A36" s="21"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="E36" s="20"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
     </row>
     <row r="37" customHeight="1" spans="1:5">
-      <c r="A37" s="21"/>
-      <c r="B37" s="19"/>
-      <c r="C37" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="E37" s="20"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
     </row>
     <row r="38" customHeight="1" spans="1:5">
-      <c r="A38" s="21"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="19"/>
-      <c r="E38" s="20"/>
+      <c r="A38" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="39" customHeight="1" spans="1:5">
-      <c r="A39" s="21"/>
-      <c r="B39" s="19"/>
-      <c r="C39" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="6"/>
     </row>
     <row r="40" customHeight="1" spans="1:5">
-      <c r="A40" s="21"/>
-      <c r="B40" s="18" t="s">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D40" s="4"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" ht="189" customHeight="1" spans="1:5">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" customHeight="1" spans="1:5">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="43" customHeight="1" spans="1:5">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="4"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" customHeight="1" spans="1:5">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" customHeight="1" spans="1:5">
+      <c r="A45" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" customHeight="1" spans="1:5">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" customHeight="1" spans="1:5">
+      <c r="A47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+    </row>
+    <row r="48" customHeight="1" spans="1:5">
+      <c r="A48" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-    </row>
-    <row r="41" customHeight="1" spans="1:5">
-      <c r="A41" s="21"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-    </row>
-    <row r="42" customHeight="1" spans="1:5">
-      <c r="A42" s="21"/>
-      <c r="B42" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="D42" s="19"/>
-      <c r="E42" s="20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" customHeight="1" spans="1:5">
-      <c r="A43" s="21"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="D43" s="19"/>
-      <c r="E43" s="20"/>
-    </row>
-    <row r="44" customHeight="1" spans="1:5">
-      <c r="A44" s="22"/>
-      <c r="B44" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-    </row>
-    <row r="45" customHeight="1" spans="1:5">
-      <c r="A45" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-    </row>
-    <row r="46" customHeight="1" spans="1:5">
-      <c r="A46" s="19"/>
-      <c r="B46" s="19"/>
-      <c r="C46" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-    </row>
-    <row r="47" customHeight="1" spans="1:5">
-      <c r="A47" s="19"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-    </row>
-    <row r="48" customHeight="1" spans="1:5">
-      <c r="A48" s="19"/>
-      <c r="B48" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C48" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="D48" s="19"/>
-      <c r="E48" s="20" t="s">
-        <v>110</v>
+      <c r="C48" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="6" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="49" customHeight="1" spans="1:5">
-      <c r="A49" s="19"/>
-      <c r="B49" s="19"/>
-      <c r="C49" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="D49" s="19"/>
-      <c r="E49" s="20"/>
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" customHeight="1" spans="1:5">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" customHeight="1" spans="1:5">
+      <c r="A51" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+    </row>
+    <row r="52" customHeight="1" spans="1:5">
+      <c r="A52" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" customHeight="1" spans="1:5">
+      <c r="A53" s="11"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" s="6"/>
+    </row>
+    <row r="54" customHeight="1" spans="1:5">
+      <c r="A54" s="11"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E54" s="6"/>
+    </row>
+    <row r="55" customHeight="1" spans="1:5">
+      <c r="A55" s="11"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="6"/>
+    </row>
+    <row r="56" customHeight="1" spans="1:5">
+      <c r="A56" s="11"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+    </row>
+    <row r="57" customHeight="1" spans="1:5">
+      <c r="A57" s="11"/>
+      <c r="B57" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" customHeight="1" spans="1:5">
+      <c r="A58" s="11"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+    </row>
+    <row r="59" customHeight="1" spans="1:5">
+      <c r="A59" s="11"/>
+      <c r="B59" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D59" s="4"/>
+      <c r="E59" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" customHeight="1" spans="1:5">
+      <c r="A60" s="11"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D60" s="4"/>
+      <c r="E60" s="6"/>
+    </row>
+    <row r="61" customHeight="1" spans="1:5">
+      <c r="A61" s="9"/>
+      <c r="B61" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" customHeight="1" spans="1:5">
+      <c r="A62" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" customHeight="1" spans="1:5">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+    </row>
+    <row r="64" customHeight="1" spans="1:5">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+    </row>
+    <row r="65" customHeight="1" spans="1:5">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D65" s="4"/>
+      <c r="E65" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="66" customHeight="1" spans="1:5">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" s="4"/>
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" customHeight="1" spans="1:5">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E67" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" customHeight="1" spans="1:5">
+      <c r="A68" s="4"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E68" s="26"/>
+    </row>
+    <row r="69" customHeight="1" spans="1:5">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E69" s="26"/>
+    </row>
+    <row r="70" ht="67" customHeight="1" spans="1:5">
+      <c r="A70" s="4"/>
+      <c r="B70" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E70" s="26"/>
+    </row>
+    <row r="71" customHeight="1" spans="1:5">
+      <c r="A71" s="4"/>
+      <c r="B71" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D71" s="4"/>
+      <c r="E71" s="10"/>
+    </row>
+    <row r="72" customHeight="1" spans="1:5">
+      <c r="A72" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+    </row>
+    <row r="73" customHeight="1" spans="1:5">
+      <c r="A73" s="22"/>
+      <c r="B73" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="C73" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+    </row>
+    <row r="74" customHeight="1" spans="1:5">
+      <c r="A74" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="C74" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+    </row>
+    <row r="75" customHeight="1" spans="1:5">
+      <c r="A75" s="22"/>
+      <c r="B75" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="C75" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="E75" s="22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="76" customHeight="1" spans="1:5">
+      <c r="A76" s="22"/>
+      <c r="B76" s="22"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="E76" s="22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="77" customHeight="1" spans="1:5">
+      <c r="A77" s="22"/>
+      <c r="B77" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C77" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="D77" s="22"/>
+      <c r="E77" s="22"/>
+    </row>
+    <row r="78" customHeight="1" spans="1:5">
+      <c r="A78" s="22"/>
+      <c r="B78" s="22"/>
+      <c r="C78" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="D78" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="E78" s="23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="79" customHeight="1" spans="1:5">
+      <c r="A79" s="22"/>
+      <c r="B79" s="22"/>
+      <c r="C79" s="23"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="23"/>
+    </row>
+    <row r="80" customHeight="1" spans="1:5">
+      <c r="A80" s="22"/>
+      <c r="B80" s="22"/>
+      <c r="C80" s="23"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="23" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="81" customHeight="1" spans="1:5">
+      <c r="A81" s="22"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D81" s="22"/>
+      <c r="E81" s="23"/>
+    </row>
+    <row r="82" customHeight="1" spans="1:5">
+      <c r="A82" s="22"/>
+      <c r="B82" s="22"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="23"/>
+    </row>
+    <row r="83" customHeight="1" spans="1:5">
+      <c r="A83" s="22"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="52">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A35:A44"/>
-    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A20:A29"/>
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A52:A61"/>
+    <mergeCell ref="A62:A71"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="A74:A83"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B35:B39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C31:C33"/>
-    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B52:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="B77:B83"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="C81:C83"/>
     <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="D78:D83"/>
     <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="E31:E33"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="E48:E50"/>
+    <mergeCell ref="E52:E55"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="E67:E71"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="E80:E83"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>